<commit_message>
Updated initial plan to be discussed within group
</commit_message>
<xml_diff>
--- a/plan_status/plan_v0.1.xlsx
+++ b/plan_status/plan_v0.1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\01_Assignment\PythonGroupAssignment\plan_status\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17A74D4F-0CC4-4E97-B737-5609115BBF85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51A6A9E6-DB4C-4215-BAA3-9A9F2D318484}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25320" yWindow="120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="69">
   <si>
     <t>Main.py</t>
   </si>
@@ -81,9 +81,6 @@
     <t>&lt;</t>
   </si>
   <si>
-    <t>Sentiment_analysis</t>
-  </si>
-  <si>
     <t>&lt;&gt;</t>
   </si>
   <si>
@@ -93,9 +90,6 @@
     <t>bool</t>
   </si>
   <si>
-    <t>blob?</t>
-  </si>
-  <si>
     <t>str</t>
   </si>
   <si>
@@ -211,6 +205,33 @@
   </si>
   <si>
     <t>to be verified</t>
+  </si>
+  <si>
+    <t>modeltype</t>
+  </si>
+  <si>
+    <t>result</t>
+  </si>
+  <si>
+    <t>score</t>
+  </si>
+  <si>
+    <t>image</t>
+  </si>
+  <si>
+    <t>blob</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>_create_blob()</t>
+  </si>
+  <si>
+    <t>_format_text()</t>
+  </si>
+  <si>
+    <t>date(KEY)</t>
   </si>
 </sst>
 </file>
@@ -453,7 +474,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -476,84 +497,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -573,15 +531,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -619,29 +568,116 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1035,8 +1071,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:L74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1053,67 +1089,67 @@
     <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="75" t="s">
+      <c r="B3" s="51" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="76"/>
+      <c r="B4" s="52"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="76"/>
+      <c r="B5" s="52"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="76"/>
+      <c r="B6" s="52"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="76"/>
+      <c r="B7" s="52"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="76"/>
+      <c r="B8" s="52"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="76"/>
+      <c r="B9" s="52"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="76"/>
+      <c r="B10" s="52"/>
     </row>
     <row r="11" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="76"/>
-      <c r="K11" s="21" t="s">
-        <v>34</v>
+      <c r="B11" s="52"/>
+      <c r="K11" s="18" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="74" t="s">
-        <v>32</v>
-      </c>
-      <c r="K12" s="83" t="s">
-        <v>61</v>
+      <c r="B12" s="50" t="s">
+        <v>30</v>
+      </c>
+      <c r="K12" s="53" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="76" t="s">
-        <v>49</v>
-      </c>
-      <c r="E13" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
-      <c r="I13" s="20"/>
-      <c r="K13" s="22" t="s">
-        <v>35</v>
+      <c r="B13" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" s="79" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="80"/>
+      <c r="G13" s="80"/>
+      <c r="H13" s="80"/>
+      <c r="I13" s="81"/>
+      <c r="K13" s="19" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="76" t="s">
-        <v>50</v>
+      <c r="B14" s="52" t="s">
+        <v>48</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="3"/>
@@ -1122,235 +1158,293 @@
       <c r="I14" s="4"/>
     </row>
     <row r="15" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="76" t="s">
-        <v>51</v>
+      <c r="B15" s="52" t="s">
+        <v>49</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="6"/>
-      <c r="K15" s="23" t="s">
-        <v>36</v>
+      <c r="K15" s="20" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="65" t="s">
-        <v>37</v>
+      <c r="B16" s="41" t="s">
+        <v>35</v>
       </c>
       <c r="E16" s="5"/>
-      <c r="F16" s="32" t="s">
+      <c r="F16" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="G16" s="33"/>
-      <c r="H16" s="34"/>
+      <c r="G16" s="77"/>
+      <c r="H16" s="78"/>
       <c r="I16" s="6"/>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" s="12"/>
       <c r="E17" s="5"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="33"/>
-      <c r="H17" s="34"/>
+      <c r="F17" s="76"/>
+      <c r="G17" s="77"/>
+      <c r="H17" s="78"/>
       <c r="I17" s="6"/>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="K17" s="62" t="s">
+        <v>50</v>
+      </c>
+      <c r="L17" s="63"/>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" s="11"/>
       <c r="E18" s="5"/>
-      <c r="F18" s="35" t="s">
+      <c r="F18" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="G18" s="36" t="s">
+      <c r="G18" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="H18" s="37" t="s">
-        <v>21</v>
+      <c r="H18" s="25" t="s">
+        <v>20</v>
       </c>
       <c r="I18" s="6"/>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="K18" s="58" t="s">
+        <v>51</v>
+      </c>
+      <c r="L18" s="59"/>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" s="11"/>
       <c r="E19" s="5"/>
-      <c r="F19" s="35" t="s">
+      <c r="F19" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="G19" s="36" t="s">
-        <v>20</v>
-      </c>
-      <c r="H19" s="37" t="s">
-        <v>26</v>
+      <c r="G19" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="H19" s="25" t="s">
+        <v>24</v>
       </c>
       <c r="I19" s="6"/>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="K19" s="58" t="s">
+        <v>52</v>
+      </c>
+      <c r="L19" s="59"/>
+    </row>
+    <row r="20" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="11"/>
       <c r="E20" s="5"/>
-      <c r="F20" s="35" t="s">
+      <c r="F20" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="G20" s="36" t="s">
+      <c r="G20" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="H20" s="37" t="s">
-        <v>23</v>
+      <c r="H20" s="25" t="s">
+        <v>21</v>
       </c>
       <c r="I20" s="6"/>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="K20" s="60"/>
+      <c r="L20" s="61"/>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B21" s="11"/>
       <c r="E21" s="5"/>
-      <c r="F21" s="35" t="s">
+      <c r="F21" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="G21" s="36" t="s">
+      <c r="G21" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="H21" s="37" t="s">
-        <v>23</v>
+      <c r="H21" s="25" t="s">
+        <v>21</v>
       </c>
       <c r="I21" s="6"/>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="K21" s="62" t="s">
+        <v>50</v>
+      </c>
+      <c r="L21" s="63"/>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B22" s="11"/>
       <c r="E22" s="5"/>
-      <c r="F22" s="35" t="s">
+      <c r="F22" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="G22" s="36" t="s">
+      <c r="G22" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="H22" s="37" t="s">
-        <v>24</v>
+      <c r="H22" s="25" t="s">
+        <v>22</v>
       </c>
       <c r="I22" s="6"/>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="K22" s="58" t="s">
+        <v>53</v>
+      </c>
+      <c r="L22" s="59"/>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B23" s="11"/>
       <c r="E23" s="5"/>
-      <c r="F23" s="35"/>
-      <c r="G23" s="36"/>
-      <c r="H23" s="37"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="25"/>
       <c r="I23" s="6"/>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="K23" s="58" t="s">
+        <v>54</v>
+      </c>
+      <c r="L23" s="59"/>
+    </row>
+    <row r="24" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="11"/>
       <c r="E24" s="5"/>
-      <c r="F24" s="35" t="s">
+      <c r="F24" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="G24" s="36" t="s">
+      <c r="G24" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="H24" s="37" t="s">
-        <v>23</v>
+      <c r="H24" s="25" t="s">
+        <v>21</v>
       </c>
       <c r="I24" s="6"/>
-    </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="K24" s="60"/>
+      <c r="L24" s="61"/>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B25" s="11"/>
       <c r="E25" s="5"/>
-      <c r="F25" s="35" t="s">
+      <c r="F25" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="G25" s="36" t="s">
+      <c r="G25" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="H25" s="37" t="s">
-        <v>23</v>
+      <c r="H25" s="25" t="s">
+        <v>21</v>
       </c>
       <c r="I25" s="6"/>
-    </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="K25" s="62" t="s">
+        <v>50</v>
+      </c>
+      <c r="L25" s="63"/>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B26" s="11"/>
       <c r="E26" s="5"/>
-      <c r="F26" s="35" t="s">
+      <c r="F26" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="G26" s="36" t="s">
+      <c r="G26" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="H26" s="37" t="s">
-        <v>24</v>
+      <c r="H26" s="25" t="s">
+        <v>22</v>
       </c>
       <c r="I26" s="6"/>
-    </row>
-    <row r="27" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K26" s="58" t="s">
+        <v>55</v>
+      </c>
+      <c r="L26" s="59"/>
+    </row>
+    <row r="27" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="11"/>
       <c r="E27" s="5"/>
-      <c r="F27" s="38"/>
-      <c r="G27" s="39"/>
-      <c r="H27" s="40"/>
+      <c r="F27" s="85"/>
+      <c r="G27" s="86"/>
+      <c r="H27" s="87"/>
       <c r="I27" s="6"/>
-    </row>
-    <row r="28" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K27" s="58" t="s">
+        <v>56</v>
+      </c>
+      <c r="L27" s="59"/>
+    </row>
+    <row r="28" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="11"/>
       <c r="E28" s="5"/>
-      <c r="F28" s="41" t="s">
-        <v>25</v>
-      </c>
-      <c r="G28" s="42"/>
-      <c r="H28" s="43"/>
+      <c r="F28" s="82" t="s">
+        <v>23</v>
+      </c>
+      <c r="G28" s="83"/>
+      <c r="H28" s="84"/>
       <c r="I28" s="6"/>
-    </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="K28" s="58"/>
+      <c r="L28" s="59"/>
+    </row>
+    <row r="29" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="11"/>
       <c r="E29" s="5"/>
-      <c r="F29" s="35" t="s">
+      <c r="F29" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="G29" s="36" t="s">
-        <v>20</v>
-      </c>
-      <c r="H29" s="37" t="s">
-        <v>23</v>
+      <c r="G29" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="H29" s="25" t="s">
+        <v>21</v>
       </c>
       <c r="I29" s="6"/>
-    </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="K29" s="60"/>
+      <c r="L29" s="61"/>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B30" s="11"/>
       <c r="E30" s="5"/>
-      <c r="F30" s="35"/>
-      <c r="G30" s="36"/>
-      <c r="H30" s="37"/>
+      <c r="F30" s="23"/>
+      <c r="G30" s="24"/>
+      <c r="H30" s="25"/>
       <c r="I30" s="6"/>
-    </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="K30" s="62" t="s">
+        <v>50</v>
+      </c>
+      <c r="L30" s="63"/>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B31" s="11"/>
       <c r="E31" s="5"/>
-      <c r="F31" s="35" t="s">
+      <c r="F31" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="G31" s="36" t="s">
-        <v>28</v>
-      </c>
-      <c r="H31" s="37" t="s">
-        <v>21</v>
+      <c r="G31" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="H31" s="25" t="s">
+        <v>20</v>
       </c>
       <c r="I31" s="6"/>
-    </row>
-    <row r="32" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K31" s="58" t="s">
+        <v>57</v>
+      </c>
+      <c r="L31" s="59"/>
+    </row>
+    <row r="32" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="13"/>
       <c r="E32" s="5"/>
-      <c r="F32" s="44" t="s">
+      <c r="F32" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="G32" s="45" t="s">
-        <v>27</v>
-      </c>
-      <c r="H32" s="46" t="s">
-        <v>21</v>
+      <c r="G32" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="H32" s="28" t="s">
+        <v>20</v>
       </c>
       <c r="I32" s="6"/>
-    </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="K32" s="58" t="s">
+        <v>58</v>
+      </c>
+      <c r="L32" s="59"/>
+    </row>
+    <row r="33" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="11"/>
       <c r="E33" s="5"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
       <c r="I33" s="6"/>
+      <c r="K33" s="60"/>
+      <c r="L33" s="61"/>
     </row>
     <row r="34" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B34" s="11"/>
@@ -1364,305 +1458,205 @@
       <c r="B35" s="13"/>
       <c r="E35" s="5"/>
       <c r="F35" s="14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
       <c r="I35" s="6"/>
     </row>
     <row r="36" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="66" t="s">
+      <c r="B36" s="42" t="s">
         <v>7</v>
       </c>
       <c r="E36" s="5"/>
-      <c r="F36" s="29" t="s">
+      <c r="F36" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="G36" s="30"/>
-      <c r="H36" s="31"/>
+      <c r="G36" s="68"/>
+      <c r="H36" s="69"/>
       <c r="I36" s="6"/>
     </row>
     <row r="37" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="11"/>
       <c r="E37" s="5"/>
-      <c r="F37" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="G37" s="25"/>
-      <c r="H37" s="26"/>
+      <c r="F37" s="73" t="s">
+        <v>65</v>
+      </c>
+      <c r="G37" s="74"/>
+      <c r="H37" s="75"/>
       <c r="I37" s="6"/>
-      <c r="K37" s="77" t="s">
-        <v>52</v>
-      </c>
-      <c r="L37" s="78"/>
     </row>
     <row r="38" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B38" s="11"/>
       <c r="E38" s="5"/>
-      <c r="F38" s="67" t="s">
-        <v>19</v>
-      </c>
-      <c r="G38" s="68" t="s">
+      <c r="F38" s="43" t="s">
+        <v>18</v>
+      </c>
+      <c r="G38" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="H38" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="H38" s="69" t="s">
-        <v>9</v>
-      </c>
       <c r="I38" s="6"/>
-      <c r="K38" s="79" t="s">
-        <v>53</v>
-      </c>
-      <c r="L38" s="80"/>
     </row>
     <row r="39" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B39" s="11"/>
       <c r="E39" s="5"/>
-      <c r="F39" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="G39" s="70" t="s">
-        <v>3</v>
-      </c>
-      <c r="H39" s="71" t="s">
+      <c r="F39" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="G39" s="46" t="s">
+        <v>60</v>
+      </c>
+      <c r="H39" s="47" t="s">
         <v>10</v>
       </c>
       <c r="I39" s="6"/>
-      <c r="K39" s="79" t="s">
-        <v>54</v>
-      </c>
-      <c r="L39" s="80"/>
-    </row>
-    <row r="40" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B40" s="11"/>
       <c r="E40" s="5"/>
-      <c r="F40" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="G40" s="72" t="s">
-        <v>5</v>
-      </c>
-      <c r="H40" s="73" t="s">
+      <c r="F40" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="G40" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="H40" s="47" t="s">
         <v>10</v>
       </c>
       <c r="I40" s="6"/>
-      <c r="K40" s="81"/>
-      <c r="L40" s="82"/>
-    </row>
-    <row r="41" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B41" s="11"/>
       <c r="E41" s="5"/>
-      <c r="F41" s="29" t="s">
+      <c r="F41" s="91" t="s">
         <v>18</v>
       </c>
-      <c r="G41" s="30"/>
-      <c r="H41" s="31"/>
+      <c r="G41" s="90" t="s">
+        <v>61</v>
+      </c>
+      <c r="H41" s="47" t="s">
+        <v>10</v>
+      </c>
       <c r="I41" s="6"/>
-      <c r="K41" s="77" t="s">
-        <v>52</v>
-      </c>
-      <c r="L41" s="78"/>
     </row>
     <row r="42" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B42" s="11"/>
       <c r="E42" s="5"/>
-      <c r="F42" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="G42" s="70" t="s">
-        <v>9</v>
-      </c>
-      <c r="H42" s="69" t="s">
-        <v>9</v>
+      <c r="F42" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="G42" s="46" t="s">
+        <v>62</v>
+      </c>
+      <c r="H42" s="47" t="s">
+        <v>10</v>
       </c>
       <c r="I42" s="6"/>
-      <c r="K42" s="79" t="s">
-        <v>55</v>
-      </c>
-      <c r="L42" s="80"/>
     </row>
     <row r="43" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B43" s="11"/>
       <c r="E43" s="5"/>
-      <c r="F43" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="G43" s="70" t="s">
-        <v>3</v>
-      </c>
-      <c r="H43" s="71" t="s">
+      <c r="F43" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="G43" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="H43" s="47" t="s">
         <v>10</v>
       </c>
       <c r="I43" s="6"/>
-      <c r="K43" s="79" t="s">
-        <v>56</v>
-      </c>
-      <c r="L43" s="80"/>
     </row>
     <row r="44" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B44" s="11"/>
       <c r="E44" s="5"/>
-      <c r="F44" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="G44" s="72" t="s">
-        <v>5</v>
-      </c>
-      <c r="H44" s="73" t="s">
-        <v>10</v>
+      <c r="F44" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="G44" s="48" t="s">
+        <v>63</v>
+      </c>
+      <c r="H44" s="49" t="s">
+        <v>64</v>
       </c>
       <c r="I44" s="6"/>
-      <c r="K44" s="81"/>
-      <c r="L44" s="82"/>
-    </row>
-    <row r="45" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="45" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B45" s="11"/>
       <c r="E45" s="5"/>
-      <c r="F45" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="G45" s="30"/>
-      <c r="H45" s="31"/>
+      <c r="F45" s="92"/>
+      <c r="G45" s="92"/>
+      <c r="H45" s="92"/>
       <c r="I45" s="6"/>
-      <c r="K45" s="77" t="s">
-        <v>52</v>
-      </c>
-      <c r="L45" s="78"/>
     </row>
     <row r="46" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B46" s="11"/>
       <c r="E46" s="5"/>
-      <c r="F46" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="G46" s="70" t="s">
-        <v>9</v>
-      </c>
-      <c r="H46" s="69" t="s">
-        <v>9</v>
-      </c>
+      <c r="F46" s="16"/>
+      <c r="G46" s="16"/>
+      <c r="H46" s="89"/>
       <c r="I46" s="6"/>
-      <c r="K46" s="79" t="s">
-        <v>57</v>
-      </c>
-      <c r="L46" s="80"/>
     </row>
     <row r="47" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B47" s="11"/>
       <c r="E47" s="5"/>
-      <c r="F47" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="G47" s="70" t="s">
-        <v>4</v>
-      </c>
-      <c r="H47" s="71" t="s">
-        <v>10</v>
-      </c>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
+      <c r="H47" s="16"/>
       <c r="I47" s="6"/>
-      <c r="K47" s="79" t="s">
-        <v>58</v>
-      </c>
-      <c r="L47" s="80"/>
     </row>
     <row r="48" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B48" s="11"/>
       <c r="E48" s="5"/>
-      <c r="F48" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="G48" s="70" t="s">
-        <v>3</v>
-      </c>
-      <c r="H48" s="71" t="s">
-        <v>10</v>
-      </c>
+      <c r="F48" s="16"/>
+      <c r="G48" s="16"/>
+      <c r="H48" s="16"/>
       <c r="I48" s="6"/>
-      <c r="K48" s="79"/>
-      <c r="L48" s="80"/>
-    </row>
-    <row r="49" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B49" s="11"/>
       <c r="E49" s="5"/>
-      <c r="F49" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="G49" s="72" t="s">
-        <v>5</v>
-      </c>
-      <c r="H49" s="73" t="s">
-        <v>10</v>
-      </c>
+      <c r="F49" s="16"/>
+      <c r="G49" s="16"/>
+      <c r="H49" s="16"/>
       <c r="I49" s="6"/>
-      <c r="K49" s="81"/>
-      <c r="L49" s="82"/>
-    </row>
-    <row r="50" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B50" s="11"/>
       <c r="E50" s="5"/>
-      <c r="F50" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="G50" s="30"/>
-      <c r="H50" s="31"/>
+      <c r="F50" s="88"/>
+      <c r="G50" s="88"/>
+      <c r="H50" s="88"/>
       <c r="I50" s="6"/>
-      <c r="K50" s="77" t="s">
-        <v>52</v>
-      </c>
-      <c r="L50" s="78"/>
-    </row>
-    <row r="51" spans="2:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B51" s="11"/>
       <c r="E51" s="5"/>
-      <c r="F51" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="G51" s="70" t="s">
-        <v>9</v>
-      </c>
-      <c r="H51" s="69" t="s">
-        <v>9</v>
-      </c>
+      <c r="F51" s="16"/>
+      <c r="G51" s="16"/>
+      <c r="H51" s="89"/>
       <c r="I51" s="6"/>
-      <c r="K51" s="79" t="s">
-        <v>59</v>
-      </c>
-      <c r="L51" s="80"/>
-    </row>
-    <row r="52" spans="2:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B52" s="11"/>
       <c r="E52" s="5"/>
-      <c r="F52" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="G52" s="70" t="s">
-        <v>6</v>
-      </c>
-      <c r="H52" s="71" t="s">
-        <v>22</v>
-      </c>
+      <c r="F52" s="16"/>
+      <c r="G52" s="16"/>
+      <c r="H52" s="16"/>
       <c r="I52" s="6"/>
-      <c r="K52" s="79" t="s">
-        <v>60</v>
-      </c>
-      <c r="L52" s="80"/>
-    </row>
-    <row r="53" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="53" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B53" s="13"/>
       <c r="E53" s="5"/>
-      <c r="F53" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="G53" s="72" t="s">
-        <v>5</v>
-      </c>
-      <c r="H53" s="73" t="s">
-        <v>10</v>
-      </c>
+      <c r="F53" s="16"/>
+      <c r="G53" s="16"/>
+      <c r="H53" s="16"/>
       <c r="I53" s="6"/>
-      <c r="K53" s="81"/>
-      <c r="L53" s="82"/>
-    </row>
-    <row r="54" spans="2:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B54" s="11"/>
       <c r="E54" s="5"/>
       <c r="F54" s="1"/>
@@ -1670,246 +1664,250 @@
       <c r="H54" s="1"/>
       <c r="I54" s="6"/>
     </row>
-    <row r="55" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B55" s="11"/>
       <c r="E55" s="5"/>
       <c r="F55" s="15" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G55" s="16"/>
       <c r="H55" s="17"/>
       <c r="I55" s="6"/>
     </row>
-    <row r="56" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="84" t="s">
+    <row r="56" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B56" s="54" t="s">
+        <v>36</v>
+      </c>
+      <c r="E56" s="5"/>
+      <c r="F56" s="70" t="s">
+        <v>11</v>
+      </c>
+      <c r="G56" s="71"/>
+      <c r="H56" s="72"/>
+      <c r="I56" s="6"/>
+    </row>
+    <row r="57" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B57" s="55" t="s">
+        <v>37</v>
+      </c>
+      <c r="E57" s="5"/>
+      <c r="F57" s="70" t="s">
+        <v>12</v>
+      </c>
+      <c r="G57" s="71"/>
+      <c r="H57" s="72"/>
+      <c r="I57" s="6"/>
+    </row>
+    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B58" s="56" t="s">
+        <v>41</v>
+      </c>
+      <c r="E58" s="5"/>
+      <c r="F58" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="G58" s="30"/>
+      <c r="H58" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="I58" s="6"/>
+    </row>
+    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B59" s="56" t="s">
         <v>38</v>
       </c>
-      <c r="E56" s="5"/>
-      <c r="F56" s="47" t="s">
-        <v>11</v>
-      </c>
-      <c r="G56" s="48"/>
-      <c r="H56" s="49"/>
-      <c r="I56" s="6"/>
-    </row>
-    <row r="57" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="85" t="s">
+      <c r="E59" s="5"/>
+      <c r="F59" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="G59" s="33"/>
+      <c r="H59" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="I59" s="6"/>
+    </row>
+    <row r="60" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B60" s="56" t="s">
         <v>39</v>
       </c>
-      <c r="E57" s="5"/>
-      <c r="F57" s="47" t="s">
-        <v>12</v>
-      </c>
-      <c r="G57" s="48"/>
-      <c r="H57" s="49"/>
-      <c r="I57" s="6"/>
-    </row>
-    <row r="58" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B58" s="86" t="s">
+      <c r="E60" s="5"/>
+      <c r="F60" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="G60" s="36"/>
+      <c r="H60" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="I60" s="6"/>
+    </row>
+    <row r="61" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B61" s="56" t="s">
+        <v>40</v>
+      </c>
+      <c r="E61" s="5"/>
+      <c r="F61" s="64" t="s">
+        <v>13</v>
+      </c>
+      <c r="G61" s="65"/>
+      <c r="H61" s="66"/>
+      <c r="I61" s="6"/>
+    </row>
+    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B62" s="56" t="s">
+        <v>41</v>
+      </c>
+      <c r="E62" s="5"/>
+      <c r="F62" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="G62" s="39"/>
+      <c r="H62" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="I62" s="6"/>
+    </row>
+    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B63" s="56" t="s">
+        <v>42</v>
+      </c>
+      <c r="E63" s="5"/>
+      <c r="F63" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="G63" s="33"/>
+      <c r="H63" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="I63" s="6"/>
+    </row>
+    <row r="64" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B64" s="56" t="s">
+        <v>67</v>
+      </c>
+      <c r="E64" s="5"/>
+      <c r="F64" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="G64" s="36"/>
+      <c r="H64" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="I64" s="6"/>
+    </row>
+    <row r="65" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B65" s="56" t="s">
         <v>43</v>
       </c>
-      <c r="E58" s="5"/>
-      <c r="F58" s="50" t="s">
+      <c r="E65" s="5"/>
+      <c r="F65" s="64" t="s">
+        <v>14</v>
+      </c>
+      <c r="G65" s="65"/>
+      <c r="H65" s="66"/>
+      <c r="I65" s="6"/>
+    </row>
+    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B66" s="56" t="s">
+        <v>41</v>
+      </c>
+      <c r="E66" s="5"/>
+      <c r="F66" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="G58" s="51"/>
-      <c r="H58" s="52" t="s">
-        <v>33</v>
-      </c>
-      <c r="I58" s="6"/>
-    </row>
-    <row r="59" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B59" s="86" t="s">
-        <v>40</v>
-      </c>
-      <c r="E59" s="5"/>
-      <c r="F59" s="53" t="s">
+      <c r="G66" s="39"/>
+      <c r="H66" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="I66" s="6"/>
+    </row>
+    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B67" s="56" t="s">
+        <v>44</v>
+      </c>
+      <c r="E67" s="5"/>
+      <c r="F67" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="G59" s="54"/>
-      <c r="H59" s="55" t="s">
+      <c r="G67" s="33"/>
+      <c r="H67" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="I67" s="6"/>
+    </row>
+    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B68" s="56"/>
+      <c r="E68" s="5"/>
+      <c r="F68" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="G68" s="33"/>
+      <c r="H68" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="I59" s="6"/>
-    </row>
-    <row r="60" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="86" t="s">
+      <c r="I68" s="6"/>
+    </row>
+    <row r="69" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B69" s="56"/>
+      <c r="E69" s="5"/>
+      <c r="F69" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="G69" s="36"/>
+      <c r="H69" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="I69" s="6"/>
+    </row>
+    <row r="70" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B70" s="56" t="s">
+        <v>45</v>
+      </c>
+      <c r="E70" s="5"/>
+      <c r="F70" s="64" t="s">
+        <v>15</v>
+      </c>
+      <c r="G70" s="65"/>
+      <c r="H70" s="66"/>
+      <c r="I70" s="6"/>
+    </row>
+    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B71" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="E60" s="5"/>
-      <c r="F60" s="56" t="s">
+      <c r="E71" s="5"/>
+      <c r="F71" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="G71" s="39"/>
+      <c r="H71" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="I71" s="6"/>
+    </row>
+    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B72" s="56" t="s">
+        <v>46</v>
+      </c>
+      <c r="E72" s="5"/>
+      <c r="F72" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="G72" s="33"/>
+      <c r="H72" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="I72" s="6"/>
+    </row>
+    <row r="73" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B73" s="57" t="s">
+        <v>66</v>
+      </c>
+      <c r="E73" s="5"/>
+      <c r="F73" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="G60" s="57"/>
-      <c r="H60" s="58" t="s">
-        <v>5</v>
-      </c>
-      <c r="I60" s="6"/>
-    </row>
-    <row r="61" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="86" t="s">
-        <v>42</v>
-      </c>
-      <c r="E61" s="5"/>
-      <c r="F61" s="59" t="s">
-        <v>13</v>
-      </c>
-      <c r="G61" s="60"/>
-      <c r="H61" s="61"/>
-      <c r="I61" s="6"/>
-    </row>
-    <row r="62" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B62" s="86" t="s">
-        <v>43</v>
-      </c>
-      <c r="E62" s="5"/>
-      <c r="F62" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="G62" s="63"/>
-      <c r="H62" s="64" t="s">
-        <v>33</v>
-      </c>
-      <c r="I62" s="6"/>
-    </row>
-    <row r="63" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B63" s="86" t="s">
-        <v>44</v>
-      </c>
-      <c r="E63" s="5"/>
-      <c r="F63" s="53" t="s">
-        <v>16</v>
-      </c>
-      <c r="G63" s="54"/>
-      <c r="H63" s="55" t="s">
-        <v>3</v>
-      </c>
-      <c r="I63" s="6"/>
-    </row>
-    <row r="64" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="86"/>
-      <c r="E64" s="5"/>
-      <c r="F64" s="56" t="s">
-        <v>17</v>
-      </c>
-      <c r="G64" s="57"/>
-      <c r="H64" s="58" t="s">
-        <v>5</v>
-      </c>
-      <c r="I64" s="6"/>
-    </row>
-    <row r="65" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B65" s="86" t="s">
-        <v>45</v>
-      </c>
-      <c r="E65" s="5"/>
-      <c r="F65" s="59" t="s">
-        <v>14</v>
-      </c>
-      <c r="G65" s="60"/>
-      <c r="H65" s="61"/>
-      <c r="I65" s="6"/>
-    </row>
-    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B66" s="86" t="s">
-        <v>43</v>
-      </c>
-      <c r="E66" s="5"/>
-      <c r="F66" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="G66" s="63"/>
-      <c r="H66" s="64" t="s">
-        <v>33</v>
-      </c>
-      <c r="I66" s="6"/>
-    </row>
-    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B67" s="86" t="s">
-        <v>46</v>
-      </c>
-      <c r="E67" s="5"/>
-      <c r="F67" s="53" t="s">
-        <v>16</v>
-      </c>
-      <c r="G67" s="54"/>
-      <c r="H67" s="55" t="s">
-        <v>4</v>
-      </c>
-      <c r="I67" s="6"/>
-    </row>
-    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B68" s="86"/>
-      <c r="E68" s="5"/>
-      <c r="F68" s="53" t="s">
-        <v>16</v>
-      </c>
-      <c r="G68" s="54"/>
-      <c r="H68" s="55" t="s">
-        <v>3</v>
-      </c>
-      <c r="I68" s="6"/>
-    </row>
-    <row r="69" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B69" s="86"/>
-      <c r="E69" s="5"/>
-      <c r="F69" s="56" t="s">
-        <v>17</v>
-      </c>
-      <c r="G69" s="57"/>
-      <c r="H69" s="58" t="s">
-        <v>5</v>
-      </c>
-      <c r="I69" s="6"/>
-    </row>
-    <row r="70" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="86" t="s">
-        <v>47</v>
-      </c>
-      <c r="E70" s="5"/>
-      <c r="F70" s="59" t="s">
-        <v>15</v>
-      </c>
-      <c r="G70" s="60"/>
-      <c r="H70" s="61"/>
-      <c r="I70" s="6"/>
-    </row>
-    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B71" s="86" t="s">
-        <v>43</v>
-      </c>
-      <c r="E71" s="5"/>
-      <c r="F71" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="G71" s="63"/>
-      <c r="H71" s="64" t="s">
-        <v>33</v>
-      </c>
-      <c r="I71" s="6"/>
-    </row>
-    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B72" s="86" t="s">
-        <v>48</v>
-      </c>
-      <c r="E72" s="5"/>
-      <c r="F72" s="53" t="s">
-        <v>16</v>
-      </c>
-      <c r="G72" s="54"/>
-      <c r="H72" s="55" t="s">
-        <v>6</v>
-      </c>
-      <c r="I72" s="6"/>
-    </row>
-    <row r="73" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B73" s="87"/>
-      <c r="E73" s="5"/>
-      <c r="F73" s="56" t="s">
-        <v>17</v>
-      </c>
-      <c r="G73" s="57"/>
-      <c r="H73" s="58" t="s">
+      <c r="G73" s="36"/>
+      <c r="H73" s="37" t="s">
         <v>5</v>
       </c>
       <c r="I73" s="6"/>
@@ -1923,24 +1921,12 @@
       <c r="I74" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="32">
-    <mergeCell ref="K51:L51"/>
-    <mergeCell ref="K52:L52"/>
-    <mergeCell ref="K53:L53"/>
-    <mergeCell ref="K38:L38"/>
-    <mergeCell ref="K39:L39"/>
-    <mergeCell ref="K40:L40"/>
-    <mergeCell ref="K45:L45"/>
-    <mergeCell ref="K41:L41"/>
-    <mergeCell ref="K37:L37"/>
-    <mergeCell ref="K50:L50"/>
-    <mergeCell ref="K42:L42"/>
-    <mergeCell ref="K43:L43"/>
-    <mergeCell ref="K44:L44"/>
-    <mergeCell ref="K46:L46"/>
-    <mergeCell ref="K47:L47"/>
-    <mergeCell ref="K48:L48"/>
-    <mergeCell ref="K49:L49"/>
+  <mergeCells count="31">
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="E13:I13"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="F27:H27"/>
     <mergeCell ref="F70:H70"/>
     <mergeCell ref="F61:H61"/>
     <mergeCell ref="F36:H36"/>
@@ -1949,13 +1935,24 @@
     <mergeCell ref="F65:H65"/>
     <mergeCell ref="F50:H50"/>
     <mergeCell ref="F37:H37"/>
-    <mergeCell ref="F41:H41"/>
     <mergeCell ref="F45:H45"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="E13:I13"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="K31:L31"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="K21:L21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
unsure if changes has been done
</commit_message>
<xml_diff>
--- a/plan_status/plan_v0.1.xlsx
+++ b/plan_status/plan_v0.1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\01_Assignment\PythonGroupAssignment\plan_status\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51A6A9E6-DB4C-4215-BAA3-9A9F2D318484}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2328F3E8-C9CC-428F-9A79-A2F98F676CD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25320" yWindow="120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="70">
   <si>
     <t>Main.py</t>
   </si>
@@ -232,6 +232,9 @@
   </si>
   <si>
     <t>date(KEY)</t>
+  </si>
+  <si>
+    <t>mohammed</t>
   </si>
 </sst>
 </file>
@@ -573,22 +576,49 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -618,6 +648,9 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -627,55 +660,25 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1071,8 +1074,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:L74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="K56" sqref="K56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1136,13 +1139,13 @@
       <c r="B13" s="52" t="s">
         <v>47</v>
       </c>
-      <c r="E13" s="79" t="s">
+      <c r="E13" s="64" t="s">
         <v>27</v>
       </c>
-      <c r="F13" s="80"/>
-      <c r="G13" s="80"/>
-      <c r="H13" s="80"/>
-      <c r="I13" s="81"/>
+      <c r="F13" s="65"/>
+      <c r="G13" s="65"/>
+      <c r="H13" s="65"/>
+      <c r="I13" s="66"/>
       <c r="K13" s="19" t="s">
         <v>33</v>
       </c>
@@ -1177,24 +1180,24 @@
         <v>35</v>
       </c>
       <c r="E16" s="5"/>
-      <c r="F16" s="76" t="s">
+      <c r="F16" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="G16" s="77"/>
-      <c r="H16" s="78"/>
+      <c r="G16" s="62"/>
+      <c r="H16" s="63"/>
       <c r="I16" s="6"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" s="12"/>
       <c r="E17" s="5"/>
-      <c r="F17" s="76"/>
-      <c r="G17" s="77"/>
-      <c r="H17" s="78"/>
+      <c r="F17" s="61"/>
+      <c r="G17" s="62"/>
+      <c r="H17" s="63"/>
       <c r="I17" s="6"/>
-      <c r="K17" s="62" t="s">
+      <c r="K17" s="87" t="s">
         <v>50</v>
       </c>
-      <c r="L17" s="63"/>
+      <c r="L17" s="88"/>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" s="11"/>
@@ -1209,10 +1212,10 @@
         <v>20</v>
       </c>
       <c r="I18" s="6"/>
-      <c r="K18" s="58" t="s">
+      <c r="K18" s="89" t="s">
         <v>51</v>
       </c>
-      <c r="L18" s="59"/>
+      <c r="L18" s="90"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" s="11"/>
@@ -1227,10 +1230,10 @@
         <v>24</v>
       </c>
       <c r="I19" s="6"/>
-      <c r="K19" s="58" t="s">
+      <c r="K19" s="89" t="s">
         <v>52</v>
       </c>
-      <c r="L19" s="59"/>
+      <c r="L19" s="90"/>
     </row>
     <row r="20" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="11"/>
@@ -1245,8 +1248,8 @@
         <v>21</v>
       </c>
       <c r="I20" s="6"/>
-      <c r="K20" s="60"/>
-      <c r="L20" s="61"/>
+      <c r="K20" s="91"/>
+      <c r="L20" s="92"/>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B21" s="11"/>
@@ -1261,10 +1264,10 @@
         <v>21</v>
       </c>
       <c r="I21" s="6"/>
-      <c r="K21" s="62" t="s">
+      <c r="K21" s="87" t="s">
         <v>50</v>
       </c>
-      <c r="L21" s="63"/>
+      <c r="L21" s="88"/>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B22" s="11"/>
@@ -1279,10 +1282,10 @@
         <v>22</v>
       </c>
       <c r="I22" s="6"/>
-      <c r="K22" s="58" t="s">
+      <c r="K22" s="89" t="s">
         <v>53</v>
       </c>
-      <c r="L22" s="59"/>
+      <c r="L22" s="90"/>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B23" s="11"/>
@@ -1291,10 +1294,10 @@
       <c r="G23" s="24"/>
       <c r="H23" s="25"/>
       <c r="I23" s="6"/>
-      <c r="K23" s="58" t="s">
+      <c r="K23" s="89" t="s">
         <v>54</v>
       </c>
-      <c r="L23" s="59"/>
+      <c r="L23" s="90"/>
     </row>
     <row r="24" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="11"/>
@@ -1309,8 +1312,8 @@
         <v>21</v>
       </c>
       <c r="I24" s="6"/>
-      <c r="K24" s="60"/>
-      <c r="L24" s="61"/>
+      <c r="K24" s="91"/>
+      <c r="L24" s="92"/>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B25" s="11"/>
@@ -1325,10 +1328,10 @@
         <v>21</v>
       </c>
       <c r="I25" s="6"/>
-      <c r="K25" s="62" t="s">
+      <c r="K25" s="87" t="s">
         <v>50</v>
       </c>
-      <c r="L25" s="63"/>
+      <c r="L25" s="88"/>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B26" s="11"/>
@@ -1343,34 +1346,34 @@
         <v>22</v>
       </c>
       <c r="I26" s="6"/>
-      <c r="K26" s="58" t="s">
+      <c r="K26" s="89" t="s">
         <v>55</v>
       </c>
-      <c r="L26" s="59"/>
+      <c r="L26" s="90"/>
     </row>
     <row r="27" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="11"/>
       <c r="E27" s="5"/>
-      <c r="F27" s="85"/>
-      <c r="G27" s="86"/>
-      <c r="H27" s="87"/>
+      <c r="F27" s="70"/>
+      <c r="G27" s="71"/>
+      <c r="H27" s="72"/>
       <c r="I27" s="6"/>
-      <c r="K27" s="58" t="s">
+      <c r="K27" s="89" t="s">
         <v>56</v>
       </c>
-      <c r="L27" s="59"/>
+      <c r="L27" s="90"/>
     </row>
     <row r="28" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="11"/>
       <c r="E28" s="5"/>
-      <c r="F28" s="82" t="s">
+      <c r="F28" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="G28" s="83"/>
-      <c r="H28" s="84"/>
+      <c r="G28" s="68"/>
+      <c r="H28" s="69"/>
       <c r="I28" s="6"/>
-      <c r="K28" s="58"/>
-      <c r="L28" s="59"/>
+      <c r="K28" s="89"/>
+      <c r="L28" s="90"/>
     </row>
     <row r="29" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="11"/>
@@ -1385,8 +1388,8 @@
         <v>21</v>
       </c>
       <c r="I29" s="6"/>
-      <c r="K29" s="60"/>
-      <c r="L29" s="61"/>
+      <c r="K29" s="91"/>
+      <c r="L29" s="92"/>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B30" s="11"/>
@@ -1395,10 +1398,10 @@
       <c r="G30" s="24"/>
       <c r="H30" s="25"/>
       <c r="I30" s="6"/>
-      <c r="K30" s="62" t="s">
+      <c r="K30" s="87" t="s">
         <v>50</v>
       </c>
-      <c r="L30" s="63"/>
+      <c r="L30" s="88"/>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B31" s="11"/>
@@ -1413,10 +1416,10 @@
         <v>20</v>
       </c>
       <c r="I31" s="6"/>
-      <c r="K31" s="58" t="s">
+      <c r="K31" s="89" t="s">
         <v>57</v>
       </c>
-      <c r="L31" s="59"/>
+      <c r="L31" s="90"/>
     </row>
     <row r="32" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="13"/>
@@ -1431,10 +1434,10 @@
         <v>20</v>
       </c>
       <c r="I32" s="6"/>
-      <c r="K32" s="58" t="s">
+      <c r="K32" s="89" t="s">
         <v>58</v>
       </c>
-      <c r="L32" s="59"/>
+      <c r="L32" s="90"/>
     </row>
     <row r="33" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="11"/>
@@ -1443,8 +1446,8 @@
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
       <c r="I33" s="6"/>
-      <c r="K33" s="60"/>
-      <c r="L33" s="61"/>
+      <c r="K33" s="91"/>
+      <c r="L33" s="92"/>
     </row>
     <row r="34" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B34" s="11"/>
@@ -1460,7 +1463,9 @@
       <c r="F35" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="G35" s="1"/>
+      <c r="G35" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="H35" s="1"/>
       <c r="I35" s="6"/>
     </row>
@@ -1469,21 +1474,21 @@
         <v>7</v>
       </c>
       <c r="E36" s="5"/>
-      <c r="F36" s="67" t="s">
+      <c r="F36" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="G36" s="68"/>
-      <c r="H36" s="69"/>
+      <c r="G36" s="77"/>
+      <c r="H36" s="78"/>
       <c r="I36" s="6"/>
     </row>
     <row r="37" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="11"/>
       <c r="E37" s="5"/>
-      <c r="F37" s="73" t="s">
+      <c r="F37" s="83" t="s">
         <v>65</v>
       </c>
-      <c r="G37" s="74"/>
-      <c r="H37" s="75"/>
+      <c r="G37" s="84"/>
+      <c r="H37" s="85"/>
       <c r="I37" s="6"/>
     </row>
     <row r="38" spans="2:12" x14ac:dyDescent="0.25">
@@ -1531,10 +1536,10 @@
     <row r="41" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B41" s="11"/>
       <c r="E41" s="5"/>
-      <c r="F41" s="91" t="s">
+      <c r="F41" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="G41" s="90" t="s">
+      <c r="G41" s="59" t="s">
         <v>61</v>
       </c>
       <c r="H41" s="47" t="s">
@@ -1587,9 +1592,9 @@
     <row r="45" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B45" s="11"/>
       <c r="E45" s="5"/>
-      <c r="F45" s="92"/>
-      <c r="G45" s="92"/>
-      <c r="H45" s="92"/>
+      <c r="F45" s="86"/>
+      <c r="G45" s="86"/>
+      <c r="H45" s="86"/>
       <c r="I45" s="6"/>
     </row>
     <row r="46" spans="2:12" x14ac:dyDescent="0.25">
@@ -1597,7 +1602,7 @@
       <c r="E46" s="5"/>
       <c r="F46" s="16"/>
       <c r="G46" s="16"/>
-      <c r="H46" s="89"/>
+      <c r="H46" s="58"/>
       <c r="I46" s="6"/>
     </row>
     <row r="47" spans="2:12" x14ac:dyDescent="0.25">
@@ -1627,9 +1632,9 @@
     <row r="50" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B50" s="11"/>
       <c r="E50" s="5"/>
-      <c r="F50" s="88"/>
-      <c r="G50" s="88"/>
-      <c r="H50" s="88"/>
+      <c r="F50" s="82"/>
+      <c r="G50" s="82"/>
+      <c r="H50" s="82"/>
       <c r="I50" s="6"/>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.25">
@@ -1637,7 +1642,7 @@
       <c r="E51" s="5"/>
       <c r="F51" s="16"/>
       <c r="G51" s="16"/>
-      <c r="H51" s="89"/>
+      <c r="H51" s="58"/>
       <c r="I51" s="6"/>
     </row>
     <row r="52" spans="2:9" x14ac:dyDescent="0.25">
@@ -1679,11 +1684,11 @@
         <v>36</v>
       </c>
       <c r="E56" s="5"/>
-      <c r="F56" s="70" t="s">
+      <c r="F56" s="79" t="s">
         <v>11</v>
       </c>
-      <c r="G56" s="71"/>
-      <c r="H56" s="72"/>
+      <c r="G56" s="80"/>
+      <c r="H56" s="81"/>
       <c r="I56" s="6"/>
     </row>
     <row r="57" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1691,11 +1696,11 @@
         <v>37</v>
       </c>
       <c r="E57" s="5"/>
-      <c r="F57" s="70" t="s">
+      <c r="F57" s="79" t="s">
         <v>12</v>
       </c>
-      <c r="G57" s="71"/>
-      <c r="H57" s="72"/>
+      <c r="G57" s="80"/>
+      <c r="H57" s="81"/>
       <c r="I57" s="6"/>
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.25">
@@ -1745,11 +1750,11 @@
         <v>40</v>
       </c>
       <c r="E61" s="5"/>
-      <c r="F61" s="64" t="s">
+      <c r="F61" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="G61" s="65"/>
-      <c r="H61" s="66"/>
+      <c r="G61" s="74"/>
+      <c r="H61" s="75"/>
       <c r="I61" s="6"/>
     </row>
     <row r="62" spans="2:9" x14ac:dyDescent="0.25">
@@ -1799,11 +1804,11 @@
         <v>43</v>
       </c>
       <c r="E65" s="5"/>
-      <c r="F65" s="64" t="s">
+      <c r="F65" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="G65" s="65"/>
-      <c r="H65" s="66"/>
+      <c r="G65" s="74"/>
+      <c r="H65" s="75"/>
       <c r="I65" s="6"/>
     </row>
     <row r="66" spans="2:9" x14ac:dyDescent="0.25">
@@ -1863,11 +1868,11 @@
         <v>45</v>
       </c>
       <c r="E70" s="5"/>
-      <c r="F70" s="64" t="s">
+      <c r="F70" s="73" t="s">
         <v>15</v>
       </c>
-      <c r="G70" s="65"/>
-      <c r="H70" s="66"/>
+      <c r="G70" s="74"/>
+      <c r="H70" s="75"/>
       <c r="I70" s="6"/>
     </row>
     <row r="71" spans="2:9" x14ac:dyDescent="0.25">
@@ -1922,11 +1927,23 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="E13:I13"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="K31:L31"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="K29:L29"/>
     <mergeCell ref="F70:H70"/>
     <mergeCell ref="F61:H61"/>
     <mergeCell ref="F36:H36"/>
@@ -1936,23 +1953,11 @@
     <mergeCell ref="F50:H50"/>
     <mergeCell ref="F37:H37"/>
     <mergeCell ref="F45:H45"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="K29:L29"/>
-    <mergeCell ref="K31:L31"/>
-    <mergeCell ref="K32:L32"/>
-    <mergeCell ref="K33:L33"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="E13:I13"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="F27:H27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>